<commit_message>
Added a couple missing data files
</commit_message>
<xml_diff>
--- a/CaliforniaNumbers.xlsx
+++ b/CaliforniaNumbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="1170" yWindow="0" windowWidth="16200" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CaliforniaNumbers" sheetId="1" r:id="rId1"/>
@@ -160,6 +160,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -237,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -253,6 +256,8 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +541,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +825,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,13 +901,13 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>3</v>
       </c>
       <c r="E4">
         <v>74</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <f t="shared" ref="F4:F12" si="0">E4/B4</f>
         <v>1.0391944838433343E-3</v>
       </c>
@@ -937,7 +942,7 @@
       <c r="E5">
         <v>65</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="8">
         <f t="shared" si="0"/>
         <v>1.2492072338708127E-3</v>
       </c>
@@ -973,7 +978,7 @@
       <c r="E6">
         <v>52</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="8">
         <f t="shared" si="0"/>
         <v>2.5072324011571841E-2</v>
       </c>
@@ -1009,7 +1014,7 @@
       <c r="E7">
         <v>37</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>9.1358024691358022E-2</v>
       </c>
@@ -1045,7 +1050,7 @@
       <c r="E8">
         <v>26</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>0.21487603305785125</v>
       </c>
@@ -1081,7 +1086,7 @@
       <c r="E9">
         <v>19</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>0.35185185185185186</v>
       </c>
@@ -1117,7 +1122,7 @@
       <c r="E10">
         <v>16</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>0.5161290322580645</v>
       </c>
@@ -1153,7 +1158,7 @@
       <c r="E11">
         <v>12</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>0.63157894736842102</v>
       </c>
@@ -1189,7 +1194,7 @@
       <c r="E12">
         <v>9</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
@@ -1225,7 +1230,7 @@
       <c r="E13">
         <v>6</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="8">
         <f>E13/B13</f>
         <v>1</v>
       </c>

</xml_diff>